<commit_message>
Update Leave Card 7/6/2023 4:34 PM
</commit_message>
<xml_diff>
--- a/AMULONG, GERONIMO.xlsx
+++ b/AMULONG, GERONIMO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14204683-3959-4AD0-B10A-C79F84BDBDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612F07FD-4AF6-4DE9-BB5C-3EC8C038EB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t>PERIOD</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>2023</t>
+  </si>
+  <si>
+    <t>SL(1-0-0)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -644,6 +647,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,6 +850,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -851,12 +863,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -2553,7 +2559,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2600,7 +2606,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A1D8C08-EA5F-4CFB-B3F2-5F53958293F6}" name="Table13" displayName="Table13" ref="A8:K77" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A1D8C08-EA5F-4CFB-B3F2-5F53958293F6}" name="Table13" displayName="Table13" ref="A8:K76" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{2434E035-034A-4C0A-8594-62557CF6BF9F}" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{C42B0E3C-44A9-45C8-94F4-B98325109E94}" name="PARTICULARS" dataDxfId="9"/>
@@ -2918,7 +2924,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2950,9 +2956,9 @@
   <dimension ref="A2:K130"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A64" activePane="bottomLeft"/>
+      <pane ySplit="3576" topLeftCell="A73" activePane="bottomLeft"/>
       <selection activeCell="I10" sqref="I10"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,7 +3119,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])</f>
-        <v>51.25</v>
+        <v>57.5</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3123,7 +3129,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])</f>
-        <v>76.25</v>
+        <v>82.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4466,7 +4472,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40">
-        <v>44927</v>
+        <v>44957</v>
       </c>
       <c r="B76" s="20"/>
       <c r="C76" s="13">
@@ -4485,15 +4491,19 @@
       <c r="K76" s="20"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="40"/>
+      <c r="A77" s="40">
+        <v>44985</v>
+      </c>
       <c r="B77" s="20"/>
-      <c r="C77" s="13"/>
+      <c r="C77" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D77" s="39"/>
       <c r="E77" s="9"/>
       <c r="F77" s="20"/>
-      <c r="G77" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G77" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H77" s="39"/>
       <c r="I77" s="9"/>
@@ -4501,15 +4511,19 @@
       <c r="K77" s="20"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="40"/>
+      <c r="A78" s="40">
+        <v>45016</v>
+      </c>
       <c r="B78" s="20"/>
-      <c r="C78" s="13"/>
+      <c r="C78" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D78" s="39"/>
       <c r="E78" s="9"/>
       <c r="F78" s="20"/>
-      <c r="G78" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G78" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H78" s="39"/>
       <c r="I78" s="9"/>
@@ -4517,15 +4531,19 @@
       <c r="K78" s="20"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A79" s="40"/>
+      <c r="A79" s="40">
+        <v>45046</v>
+      </c>
       <c r="B79" s="20"/>
-      <c r="C79" s="13"/>
+      <c r="C79" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G79" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H79" s="39"/>
       <c r="I79" s="9"/>
@@ -4533,15 +4551,19 @@
       <c r="K79" s="20"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A80" s="40"/>
+      <c r="A80" s="40">
+        <v>45077</v>
+      </c>
       <c r="B80" s="20"/>
-      <c r="C80" s="13"/>
+      <c r="C80" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D80" s="39"/>
       <c r="E80" s="9"/>
       <c r="F80" s="20"/>
-      <c r="G80" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G80" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H80" s="39"/>
       <c r="I80" s="9"/>
@@ -4549,15 +4571,19 @@
       <c r="K80" s="20"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A81" s="40"/>
+      <c r="A81" s="40">
+        <v>45107</v>
+      </c>
       <c r="B81" s="20"/>
-      <c r="C81" s="13"/>
+      <c r="C81" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D81" s="39"/>
       <c r="E81" s="9"/>
       <c r="F81" s="20"/>
-      <c r="G81" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G81" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H81" s="39"/>
       <c r="I81" s="9"/>
@@ -4565,7 +4591,9 @@
       <c r="K81" s="20"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="40"/>
+      <c r="A82" s="40">
+        <v>45138</v>
+      </c>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
       <c r="D82" s="39"/>
@@ -4581,7 +4609,9 @@
       <c r="K82" s="20"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" s="40"/>
+      <c r="A83" s="40">
+        <v>45169</v>
+      </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
       <c r="D83" s="39"/>
@@ -4597,7 +4627,9 @@
       <c r="K83" s="20"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A84" s="40"/>
+      <c r="A84" s="40">
+        <v>45199</v>
+      </c>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
       <c r="D84" s="39"/>
@@ -4613,7 +4645,9 @@
       <c r="K84" s="20"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="40"/>
+      <c r="A85" s="40">
+        <v>45230</v>
+      </c>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
       <c r="D85" s="39"/>
@@ -4629,7 +4663,9 @@
       <c r="K85" s="20"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="40"/>
+      <c r="A86" s="40">
+        <v>45260</v>
+      </c>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
       <c r="D86" s="39"/>
@@ -4645,7 +4681,9 @@
       <c r="K86" s="20"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="40"/>
+      <c r="A87" s="40">
+        <v>45291</v>
+      </c>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
       <c r="D87" s="39"/>
@@ -4661,7 +4699,9 @@
       <c r="K87" s="20"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A88" s="40"/>
+      <c r="A88" s="40">
+        <v>45322</v>
+      </c>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
       <c r="D88" s="39"/>
@@ -4677,7 +4717,9 @@
       <c r="K88" s="20"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A89" s="40"/>
+      <c r="A89" s="40">
+        <v>45351</v>
+      </c>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
       <c r="D89" s="39"/>
@@ -4693,7 +4735,9 @@
       <c r="K89" s="20"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="40"/>
+      <c r="A90" s="40">
+        <v>45382</v>
+      </c>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
       <c r="D90" s="39"/>
@@ -4709,7 +4753,9 @@
       <c r="K90" s="20"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A91" s="40"/>
+      <c r="A91" s="40">
+        <v>45412</v>
+      </c>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
       <c r="D91" s="39"/>
@@ -4725,7 +4771,9 @@
       <c r="K91" s="20"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="40"/>
+      <c r="A92" s="40">
+        <v>45443</v>
+      </c>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
       <c r="D92" s="39"/>
@@ -4741,7 +4789,9 @@
       <c r="K92" s="20"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="40"/>
+      <c r="A93" s="40">
+        <v>45473</v>
+      </c>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
       <c r="D93" s="39"/>
@@ -4757,7 +4807,9 @@
       <c r="K93" s="20"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A94" s="40"/>
+      <c r="A94" s="40">
+        <v>45504</v>
+      </c>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
       <c r="D94" s="39"/>
@@ -4773,7 +4825,9 @@
       <c r="K94" s="20"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A95" s="40"/>
+      <c r="A95" s="40">
+        <v>45535</v>
+      </c>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
       <c r="D95" s="39"/>
@@ -4789,7 +4843,9 @@
       <c r="K95" s="20"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96" s="40"/>
+      <c r="A96" s="40">
+        <v>45565</v>
+      </c>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
       <c r="D96" s="39"/>
@@ -4805,7 +4861,9 @@
       <c r="K96" s="20"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="40"/>
+      <c r="A97" s="40">
+        <v>45596</v>
+      </c>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
       <c r="D97" s="39"/>
@@ -4821,7 +4879,9 @@
       <c r="K97" s="20"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A98" s="40"/>
+      <c r="A98" s="40">
+        <v>45626</v>
+      </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
       <c r="D98" s="39"/>
@@ -4837,7 +4897,9 @@
       <c r="K98" s="20"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="40"/>
+      <c r="A99" s="40">
+        <v>45657</v>
+      </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
       <c r="D99" s="39"/>
@@ -5393,12 +5455,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K77"/>
+  <dimension ref="A2:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A11" activePane="bottomLeft"/>
+      <pane ySplit="3576" topLeftCell="A14" activePane="bottomLeft"/>
       <selection activeCell="F5" sqref="F5"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5569,7 +5631,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>176.25</v>
+        <v>175.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -5752,7 +5814,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="13"/>
@@ -5769,12 +5831,16 @@
       <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="20"/>
+      <c r="A19" s="40">
+        <v>44866</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="39">
+        <v>3</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="20"/>
       <c r="G19" s="13" t="str">
@@ -5784,19 +5850,17 @@
       <c r="H19" s="39"/>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="20"/>
+      <c r="K19" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="40">
-        <v>44866</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="A20" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="20"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="39">
-        <v>3</v>
-      </c>
+      <c r="D20" s="39"/>
       <c r="E20" s="9"/>
       <c r="F20" s="20"/>
       <c r="G20" s="13" t="str">
@@ -5806,13 +5870,15 @@
       <c r="H20" s="39"/>
       <c r="I20" s="9"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="40">
+        <v>45108</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="C21" s="13"/>
       <c r="D21" s="39"/>
       <c r="E21" s="9"/>
@@ -5821,10 +5887,14 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H21" s="39"/>
+      <c r="H21" s="39">
+        <v>1</v>
+      </c>
       <c r="I21" s="9"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="60">
+        <v>45106</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
@@ -6691,50 +6761,34 @@
       <c r="K75" s="20"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="40"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="39"/>
+      <c r="A76" s="41"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="43"/>
       <c r="E76" s="9"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="13" t="str">
+      <c r="F76" s="15"/>
+      <c r="G76" s="42" t="str">
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H76" s="39"/>
+      <c r="H76" s="43"/>
       <c r="I76" s="9"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="20"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="41"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="42"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="42" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H77" s="43"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="15"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{9A68AE10-7817-4AB0-BD1F-FE53B2F408E7}">

</xml_diff>